<commit_message>
color change on plots
</commit_message>
<xml_diff>
--- a/3 TP Analysis/01 - Data/Ascidian_transect_percent_cover.xlsx
+++ b/3 TP Analysis/01 - Data/Ascidian_transect_percent_cover.xlsx
@@ -557,7 +557,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>7.75815779329597</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -577,7 +577,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>4.55041037357085</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -597,7 +597,7 @@
         <v>4.6</v>
       </c>
       <c r="F4" t="n">
-        <v>5.014131265302</v>
+        <v>2.33428552000155</v>
       </c>
     </row>
     <row r="5">
@@ -617,7 +617,7 @@
         <v>0.3</v>
       </c>
       <c r="F5" t="n">
-        <v>6.99723049269504</v>
+        <v>0.213437474581095</v>
       </c>
     </row>
     <row r="6">
@@ -637,7 +637,7 @@
         <v>0.9</v>
       </c>
       <c r="F6" t="n">
-        <v>4.21605543805939</v>
+        <v>0.690410505906933</v>
       </c>
     </row>
     <row r="7">
@@ -657,7 +657,7 @@
         <v>0.6</v>
       </c>
       <c r="F7" t="n">
-        <v>4.58355891700751</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="8">
@@ -677,7 +677,7 @@
         <v>0.3</v>
       </c>
       <c r="F8" t="n">
-        <v>5.15680360851469</v>
+        <v>0.213437474581095</v>
       </c>
     </row>
     <row r="9">
@@ -697,7 +697,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>6.0130285502132</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -717,7 +717,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>6.97586005140514</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -737,7 +737,7 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>5.09881370855691</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -757,7 +757,7 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>4.51006419159924</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -777,7 +777,7 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>5.63265391475961</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -797,7 +797,7 @@
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>6.67806202020309</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -817,7 +817,7 @@
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>5.95595977069384</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -837,7 +837,7 @@
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>5.22096320520682</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -857,7 +857,7 @@
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>5.31975992682117</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -877,7 +877,7 @@
         <v>0.8</v>
       </c>
       <c r="F18" t="n">
-        <v>4.49260022594081</v>
+        <v>0.442216638714053</v>
       </c>
     </row>
     <row r="19">
@@ -897,7 +897,7 @@
         <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>8.25544339687532</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -917,7 +917,7 @@
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>4.63448560145821</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -937,7 +937,7 @@
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>4.97793588538586</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -957,7 +957,7 @@
         <v>0.1</v>
       </c>
       <c r="F22" t="n">
-        <v>4.48331612278123</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="23">
@@ -977,7 +977,7 @@
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>5.70008392834031</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -997,7 +997,7 @@
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>9.95622982587681</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1017,7 +1017,7 @@
         <v>0.1</v>
       </c>
       <c r="F25" t="n">
-        <v>4.64932624881297</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="26">
@@ -1037,7 +1037,7 @@
         <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>5.2613223001142</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1057,7 +1057,7 @@
         <v>0.3</v>
       </c>
       <c r="F27" t="n">
-        <v>4.45893125101011</v>
+        <v>0.213437474581095</v>
       </c>
     </row>
     <row r="28">
@@ -1077,7 +1077,7 @@
         <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>6.62800130013324</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1097,7 +1097,7 @@
         <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>6.13366041800953</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1117,7 +1117,7 @@
         <v>0.1</v>
       </c>
       <c r="F30" t="n">
-        <v>6.24729818144622</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="31">
@@ -1137,7 +1137,7 @@
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>5.20345623505411</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -1157,7 +1157,7 @@
         <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>6.32203914985867</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1177,7 +1177,7 @@
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>3.95173817046388</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1197,7 +1197,7 @@
         <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>5.2479743299583</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -1217,7 +1217,7 @@
         <v>0.1</v>
       </c>
       <c r="F35" t="n">
-        <v>3.70264336673606</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="36">
@@ -1237,7 +1237,7 @@
         <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>7.70211811495968</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -1257,7 +1257,7 @@
         <v>0</v>
       </c>
       <c r="F37" t="n">
-        <v>5.40700277532254</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -1277,7 +1277,7 @@
         <v>0.3</v>
       </c>
       <c r="F38" t="n">
-        <v>5.79792693901221</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="39">
@@ -1297,7 +1297,7 @@
         <v>0</v>
       </c>
       <c r="F39" t="n">
-        <v>7.95577086921543</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -1317,7 +1317,7 @@
         <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>7.00296453979877</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -1337,7 +1337,7 @@
         <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>5.0939355131711</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -1357,7 +1357,7 @@
         <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>4.79665521322597</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -1377,7 +1377,7 @@
         <v>0</v>
       </c>
       <c r="F43" t="n">
-        <v>5.73876788083674</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -1397,7 +1397,7 @@
         <v>1</v>
       </c>
       <c r="F44" t="n">
-        <v>4.32763870836319</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -1417,7 +1417,7 @@
         <v>0</v>
       </c>
       <c r="F45" t="n">
-        <v>7.86593295385664</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -1437,7 +1437,7 @@
         <v>0.6</v>
       </c>
       <c r="F46" t="n">
-        <v>4.94928290104414</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="47">
@@ -1457,7 +1457,7 @@
         <v>0</v>
       </c>
       <c r="F47" t="n">
-        <v>6.2337220120452</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -1477,7 +1477,7 @@
         <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>5.39105340264066</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -1497,7 +1497,7 @@
         <v>0.1</v>
       </c>
       <c r="F49" t="n">
-        <v>6.09007490476751</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="50">
@@ -1517,7 +1517,7 @@
         <v>0</v>
       </c>
       <c r="F50" t="n">
-        <v>6.0216509001527</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -1537,7 +1537,7 @@
         <v>0</v>
       </c>
       <c r="F51" t="n">
-        <v>4.71673864622475</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -1557,7 +1557,7 @@
         <v>0</v>
       </c>
       <c r="F52" t="n">
-        <v>5.53404725425666</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -1577,7 +1577,7 @@
         <v>0</v>
       </c>
       <c r="F53" t="n">
-        <v>7.46700974740901</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -1597,7 +1597,7 @@
         <v>0.1</v>
       </c>
       <c r="F54" t="n">
-        <v>5.11605437282277</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="55">
@@ -1617,7 +1617,7 @@
         <v>1.18181818181818</v>
       </c>
       <c r="F55" t="n">
-        <v>7.44431081387129</v>
+        <v>1.18181818181818</v>
       </c>
     </row>
     <row r="56">
@@ -1637,7 +1637,7 @@
         <v>1.4</v>
       </c>
       <c r="F56" t="n">
-        <v>4.1489437894362</v>
+        <v>0.90921211313239</v>
       </c>
     </row>
     <row r="57">
@@ -1657,7 +1657,7 @@
         <v>0</v>
       </c>
       <c r="F57" t="n">
-        <v>6.71735820353269</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -1677,7 +1677,7 @@
         <v>0</v>
       </c>
       <c r="F58" t="n">
-        <v>5.68493243496556</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -1697,7 +1697,7 @@
         <v>0.1</v>
       </c>
       <c r="F59" t="n">
-        <v>4.36292602009135</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="60">
@@ -1717,7 +1717,7 @@
         <v>0.272727272727273</v>
       </c>
       <c r="F60" t="n">
-        <v>6.54704627422513</v>
+        <v>0.272727272727273</v>
       </c>
     </row>
     <row r="61">
@@ -1737,7 +1737,7 @@
         <v>0</v>
       </c>
       <c r="F61" t="n">
-        <v>4.54746868955706</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -1757,7 +1757,7 @@
         <v>0.818181818181818</v>
       </c>
       <c r="F62" t="n">
-        <v>4.30606427872281</v>
+        <v>0.263479577203444</v>
       </c>
     </row>
     <row r="63">
@@ -1777,7 +1777,7 @@
         <v>0.2</v>
       </c>
       <c r="F63" t="n">
-        <v>5.86591956522411</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="64">
@@ -1797,7 +1797,7 @@
         <v>0</v>
       </c>
       <c r="F64" t="n">
-        <v>4.81835162121643</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -1817,7 +1817,7 @@
         <v>0</v>
       </c>
       <c r="F65" t="n">
-        <v>5.96535005130193</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -1837,7 +1837,7 @@
         <v>0</v>
       </c>
       <c r="F66" t="n">
-        <v>4.8865303654378</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -1857,7 +1857,7 @@
         <v>0.1</v>
       </c>
       <c r="F67" t="n">
-        <v>5.35781994545368</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="68">
@@ -1877,7 +1877,7 @@
         <v>1.5</v>
       </c>
       <c r="F68" t="n">
-        <v>4.06555464455974</v>
+        <v>0.703167436990966</v>
       </c>
     </row>
     <row r="69">
@@ -1897,7 +1897,7 @@
         <v>0</v>
       </c>
       <c r="F69" t="n">
-        <v>4.40471478596277</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -1917,7 +1917,7 @@
         <v>0</v>
       </c>
       <c r="F70" t="n">
-        <v>4.53683824205447</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -1937,7 +1937,7 @@
         <v>0.1</v>
       </c>
       <c r="F71" t="n">
-        <v>3.99883470680468</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="72">
@@ -1957,7 +1957,7 @@
         <v>0.2</v>
       </c>
       <c r="F72" t="n">
-        <v>3.9930649758343</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="73">
@@ -1977,7 +1977,7 @@
         <v>0.4</v>
       </c>
       <c r="F73" t="n">
-        <v>4.75533164062673</v>
+        <v>0.221108319357027</v>
       </c>
     </row>
     <row r="74">
@@ -1997,7 +1997,7 @@
         <v>0.7</v>
       </c>
       <c r="F74" t="n">
-        <v>3.93009910973574</v>
+        <v>0.517472489875334</v>
       </c>
     </row>
     <row r="75">
@@ -2017,7 +2017,7 @@
         <v>0</v>
       </c>
       <c r="F75" t="n">
-        <v>4.75503956182994</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -2037,7 +2037,7 @@
         <v>0</v>
       </c>
       <c r="F76" t="n">
-        <v>5.68371075101773</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -2057,7 +2057,7 @@
         <v>0.7</v>
       </c>
       <c r="F77" t="n">
-        <v>5.27279296758486</v>
+        <v>0.517472489875334</v>
       </c>
     </row>
     <row r="78">
@@ -2077,7 +2077,7 @@
         <v>0</v>
       </c>
       <c r="F78" t="n">
-        <v>5.63612959309165</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -2097,7 +2097,7 @@
         <v>1.4</v>
       </c>
       <c r="F79" t="n">
-        <v>3.69129774095042</v>
+        <v>1.03494497975067</v>
       </c>
     </row>
     <row r="80">
@@ -2117,7 +2117,7 @@
         <v>0</v>
       </c>
       <c r="F80" t="n">
-        <v>5.38055770664788</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -2137,7 +2137,7 @@
         <v>0</v>
       </c>
       <c r="F81" t="n">
-        <v>5.93411615726396</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -2157,7 +2157,7 @@
         <v>0</v>
       </c>
       <c r="F82" t="n">
-        <v>4.82981033801893</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -2177,7 +2177,7 @@
         <v>0.2</v>
       </c>
       <c r="F83" t="n">
-        <v>4.43488207423215</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="84">
@@ -2197,7 +2197,7 @@
         <v>0</v>
       </c>
       <c r="F84" t="n">
-        <v>4.0538200243873</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -2217,7 +2217,7 @@
         <v>0</v>
       </c>
       <c r="F85" t="n">
-        <v>5.53289266429125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -2237,7 +2237,7 @@
         <v>0</v>
       </c>
       <c r="F86" t="n">
-        <v>4.01332656576272</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -2257,7 +2257,7 @@
         <v>0</v>
       </c>
       <c r="F87" t="n">
-        <v>11.088401953936</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88">
@@ -2277,7 +2277,7 @@
         <v>5.9</v>
       </c>
       <c r="F88" t="n">
-        <v>4.2944875662633</v>
+        <v>2.9152853872115</v>
       </c>
     </row>
     <row r="89">
@@ -2297,7 +2297,7 @@
         <v>4.4</v>
       </c>
       <c r="F89" t="n">
-        <v>4.88377257536643</v>
+        <v>1.43139403690559</v>
       </c>
     </row>
     <row r="90">
@@ -2317,7 +2317,7 @@
         <v>8.6</v>
       </c>
       <c r="F90" t="n">
-        <v>4.71650307267661</v>
+        <v>3.91918358845308</v>
       </c>
     </row>
     <row r="91">
@@ -2337,7 +2337,7 @@
         <v>0</v>
       </c>
       <c r="F91" t="n">
-        <v>5.99644441973845</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92">
@@ -2357,7 +2357,7 @@
         <v>0</v>
       </c>
       <c r="F92" t="n">
-        <v>3.73148929325531</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93">
@@ -2377,7 +2377,7 @@
         <v>0</v>
       </c>
       <c r="F93" t="n">
-        <v>4.52856503040068</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94">
@@ -2397,7 +2397,7 @@
         <v>0</v>
       </c>
       <c r="F94" t="n">
-        <v>5.19271510131807</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95">
@@ -2417,7 +2417,7 @@
         <v>0.1</v>
       </c>
       <c r="F95" t="n">
-        <v>4.03967973305793</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="96">
@@ -2437,7 +2437,7 @@
         <v>0</v>
       </c>
       <c r="F96" t="n">
-        <v>6.89549862117076</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97">
@@ -2457,7 +2457,7 @@
         <v>0</v>
       </c>
       <c r="F97" t="n">
-        <v>5.77805821968968</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98">
@@ -2477,7 +2477,7 @@
         <v>0</v>
       </c>
       <c r="F98" t="n">
-        <v>6.55011544521766</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99">
@@ -2497,7 +2497,7 @@
         <v>0</v>
       </c>
       <c r="F99" t="n">
-        <v>4.01775381015467</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100">
@@ -2517,7 +2517,7 @@
         <v>0</v>
       </c>
       <c r="F100" t="n">
-        <v>5.34120368363943</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101">
@@ -2537,7 +2537,7 @@
         <v>0</v>
       </c>
       <c r="F101" t="n">
-        <v>4.71063938938125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102">
@@ -2557,7 +2557,7 @@
         <v>0</v>
       </c>
       <c r="F102" t="n">
-        <v>5.69459891389406</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103">
@@ -2577,7 +2577,7 @@
         <v>0</v>
       </c>
       <c r="F103" t="n">
-        <v>4.08661243997616</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104">
@@ -2597,7 +2597,7 @@
         <v>0</v>
       </c>
       <c r="F104" t="n">
-        <v>5.63191413199131</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105">
@@ -2617,7 +2617,7 @@
         <v>0.3</v>
       </c>
       <c r="F105" t="n">
-        <v>4.60366534056302</v>
+        <v>0.152752523165195</v>
       </c>
     </row>
     <row r="106">
@@ -2637,7 +2637,7 @@
         <v>0</v>
       </c>
       <c r="F106" t="n">
-        <v>6.16038969827136</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107">
@@ -2657,7 +2657,7 @@
         <v>0</v>
       </c>
       <c r="F107" t="n">
-        <v>3.95560237175791</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108">
@@ -2677,7 +2677,7 @@
         <v>0</v>
       </c>
       <c r="F108" t="n">
-        <v>4.98161744272671</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109">
@@ -2697,7 +2697,7 @@
         <v>0</v>
       </c>
       <c r="F109" t="n">
-        <v>3.82104713849069</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110">
@@ -2717,7 +2717,7 @@
         <v>0</v>
       </c>
       <c r="F110" t="n">
-        <v>7.73093433415472</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111">
@@ -2737,7 +2737,7 @@
         <v>5</v>
       </c>
       <c r="F111" t="n">
-        <v>5.26564980807066</v>
+        <v>3.13758576686669</v>
       </c>
     </row>
     <row r="112">
@@ -2757,7 +2757,7 @@
         <v>0</v>
       </c>
       <c r="F112" t="n">
-        <v>8.59477303113876</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113">
@@ -2777,7 +2777,7 @@
         <v>0</v>
       </c>
       <c r="F113" t="n">
-        <v>7.95842398629773</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114">
@@ -2797,7 +2797,7 @@
         <v>0.5</v>
       </c>
       <c r="F114" t="n">
-        <v>4.75471825443026</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="115">
@@ -2817,7 +2817,7 @@
         <v>0</v>
       </c>
       <c r="F115" t="n">
-        <v>7.74154457105809</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116">
@@ -2837,7 +2837,7 @@
         <v>0.3</v>
       </c>
       <c r="F116" t="n">
-        <v>6.85075917213325</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="117">
@@ -2857,7 +2857,7 @@
         <v>0.2</v>
       </c>
       <c r="F117" t="n">
-        <v>3.90019388565223</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="118">
@@ -2877,7 +2877,7 @@
         <v>0</v>
       </c>
       <c r="F118" t="n">
-        <v>3.71182212084444</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119">
@@ -2897,7 +2897,7 @@
         <v>0.2</v>
       </c>
       <c r="F119" t="n">
-        <v>4.15800581356965</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="120">
@@ -2917,7 +2917,7 @@
         <v>0</v>
       </c>
       <c r="F120" t="n">
-        <v>4.17886362957298</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121">
@@ -2937,7 +2937,7 @@
         <v>0</v>
       </c>
       <c r="F121" t="n">
-        <v>4.14351717359796</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122">
@@ -2957,7 +2957,7 @@
         <v>0</v>
       </c>
       <c r="F122" t="n">
-        <v>5.3292808678002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123">
@@ -2977,7 +2977,7 @@
         <v>0</v>
       </c>
       <c r="F123" t="n">
-        <v>4.41730952693946</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124">
@@ -2997,7 +2997,7 @@
         <v>0</v>
       </c>
       <c r="F124" t="n">
-        <v>4.15890759042312</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125">
@@ -3017,7 +3017,7 @@
         <v>0</v>
       </c>
       <c r="F125" t="n">
-        <v>4.34793835067088</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126">
@@ -3037,7 +3037,7 @@
         <v>0</v>
       </c>
       <c r="F126" t="n">
-        <v>4.03293539512283</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127">
@@ -3057,7 +3057,7 @@
         <v>0.1</v>
       </c>
       <c r="F127" t="n">
-        <v>4.40017185410741</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="128">
@@ -3077,7 +3077,7 @@
         <v>0</v>
       </c>
       <c r="F128" t="n">
-        <v>6.65554164346533</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129">
@@ -3097,7 +3097,7 @@
         <v>0</v>
       </c>
       <c r="F129" t="n">
-        <v>5.40235145418806</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130">
@@ -3117,7 +3117,7 @@
         <v>0</v>
       </c>
       <c r="F130" t="n">
-        <v>5.25289455772414</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>